<commit_message>
1. fix monthly report stat bug
</commit_message>
<xml_diff>
--- a/report_template/monthlyReport.xlsx
+++ b/report_template/monthlyReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\webApp\Datalogger2\report_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\Datalogger2\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16C8A42-801A-4E8D-A224-B311970982A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF854673-E0D1-44EB-B81C-3524E383C0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12675" yWindow="3990" windowWidth="23580" windowHeight="17010" xr2:uid="{1FF98DE7-DF0E-49E7-AD88-0362929A6F74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FF98DE7-DF0E-49E7-AD88-0362929A6F74}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,14 +95,23 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -175,26 +184,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,7 +523,7 @@
   <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -523,16 +532,16 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -542,76 +551,76 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="3"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="3"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="3"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+      <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+      <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>

</xml_diff>

<commit_message>
1. monthly report fix 2. 九份子排版調整 3. 趨勢圖bug fix
</commit_message>
<xml_diff>
--- a/report_template/monthlyReport.xlsx
+++ b/report_template/monthlyReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\Datalogger2\report_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\Datalogger2\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF854673-E0D1-44EB-B81C-3524E383C0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F99C8-BA1A-4E6F-ADD6-71658C8F1BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FF98DE7-DF0E-49E7-AD88-0362929A6F74}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{1FF98DE7-DF0E-49E7-AD88-0362929A6F74}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -34,24 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>底色說明</t>
-  </si>
-  <si>
-    <t>校正</t>
-  </si>
-  <si>
-    <t>維修</t>
-  </si>
-  <si>
-    <t>異常</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>人工註記</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>日期</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -117,7 +100,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,19 +114,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,29 +151,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -523,124 +488,118 @@
   <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.69140625" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
     </row>
   </sheetData>

</xml_diff>